<commit_message>
'Sgene linked' database missing 'Name' column resolved. Data dictionary formats updated.
</commit_message>
<xml_diff>
--- a/data_dictionary/EAVEII_data_dictionary.xlsx
+++ b/data_dictionary/EAVEII_data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/rmulholl_ed_ac_uk/Documents/BREATHE/EAVE II/Data Dictionary/EAVE_II_data_dictionary/EAVE-II-data-dictionary/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DE38BD1-B32E-407D-83DD-C871228D0D2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EFE3BEB-76FE-49A5-97C3-61BA92A688DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="4" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="491">
   <si>
     <t>Name</t>
   </si>
@@ -1302,9 +1302,6 @@
     <t>Time (days) from +ve test to admission</t>
   </si>
   <si>
-    <t>Time (days) from +ve test to dearh</t>
-  </si>
-  <si>
     <t>Quintile of scottish index of multiple deprivation (from postcode of residence)</t>
   </si>
   <si>
@@ -1522,6 +1519,54 @@
   </si>
   <si>
     <t>HPS case-control files</t>
+  </si>
+  <si>
+    <t>Specimen Date</t>
+  </si>
+  <si>
+    <t>Sub Lab</t>
+  </si>
+  <si>
+    <t>COVID result</t>
+  </si>
+  <si>
+    <t>Date of NRS death record</t>
+  </si>
+  <si>
+    <t>Death within 28 days of positive test</t>
+  </si>
+  <si>
+    <t>SIMD Quintile 2020</t>
+  </si>
+  <si>
+    <t>Admission to hospital date</t>
+  </si>
+  <si>
+    <t>Discharge from hospital date</t>
+  </si>
+  <si>
+    <t>COVID admission</t>
+  </si>
+  <si>
+    <t>Time from positive test to admission</t>
+  </si>
+  <si>
+    <t>COVID death</t>
+  </si>
+  <si>
+    <t>Time from poistive test to death</t>
+  </si>
+  <si>
+    <t>Time (days) from +ve test to death</t>
+  </si>
+  <si>
+    <t>Days of…</t>
+  </si>
+  <si>
+    <t>True S Gene Dropout</t>
+  </si>
+  <si>
+    <t>New patient since last linkage</t>
   </si>
 </sst>
 </file>
@@ -1962,7 +2007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2036,7 +2081,7 @@
         <v>246</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -2048,7 +2093,7 @@
         <v>200</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2059,7 +2104,7 @@
         <v>247</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>66</v>
@@ -2068,10 +2113,10 @@
         <v>271</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2105,13 +2150,13 @@
         <v>252</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>273</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -2122,7 +2167,7 @@
         <v>254</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>122</v>
@@ -2131,24 +2176,24 @@
         <v>273</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>255</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>65</v>
@@ -2156,30 +2201,30 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>469</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>264</v>
@@ -2190,7 +2235,7 @@
     </row>
     <row r="11" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>263</v>
@@ -2210,7 +2255,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>273</v>
@@ -2230,7 +2275,7 @@
         <v>273</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -2263,104 +2308,117 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="96.625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.25" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="16"/>
+    <col min="1" max="1" width="9" style="16"/>
+    <col min="2" max="2" width="25.875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="96.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.25" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="23"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3" s="16" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>384</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4" s="16" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>71</v>
       </c>
@@ -2368,289 +2426,337 @@
         <v>16</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5" s="16" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>385</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="16" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>401</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="16" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>386</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>478</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="16" t="s">
         <v>397</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="E10" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>387</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>407</v>
+        <v>480</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F11" s="22" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>388</v>
       </c>
       <c r="B12" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E12" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F12" s="16" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>389</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F13" s="16" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>390</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>442</v>
+        <v>483</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>441</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" s="16" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>391</v>
       </c>
       <c r="B15" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>405</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>443</v>
+      <c r="E15" s="18" t="s">
+        <v>417</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>392</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>428</v>
+        <v>485</v>
       </c>
       <c r="C16" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="16" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>393</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>406</v>
+        <v>486</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>487</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>444</v>
+      <c r="E17" s="18" t="s">
+        <v>417</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>443</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>448</v>
-      </c>
-      <c r="C18" s="16" t="s">
+      <c r="B18" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>447</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>447</v>
+      <c r="E18" s="18" t="s">
+        <v>417</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>395</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>408</v>
-      </c>
-      <c r="C19" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="E19" s="17" t="s">
         <v>398</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="16" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>396</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>445</v>
+        <v>490</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>418</v>
-      </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>416</v>
+      <c r="G20" s="16" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -2710,29 +2816,29 @@
     </row>
     <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>461</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>462</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>466</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2960,7 +3066,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -2983,7 +3089,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -3150,7 +3256,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -3521,7 +3627,7 @@
         <v>203</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>227</v>
@@ -3541,7 +3647,7 @@
         <v>204</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>227</v>
@@ -3628,16 +3734,16 @@
         <v>228</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>290</v>
       </c>
       <c r="G20" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>416</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3901,7 +4007,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3991,7 +4097,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>92</v>
@@ -4003,7 +4109,7 @@
         <v>227</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>110</v>
@@ -4025,7 +4131,7 @@
         <v>111</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>112</v>
@@ -4033,12 +4139,12 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>282</v>
@@ -4058,7 +4164,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4083,7 +4189,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -4106,7 +4212,7 @@
         <v>290</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -4123,16 +4229,16 @@
         <v>111</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>290</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -4149,13 +4255,13 @@
         <v>111</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>290</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -4218,7 +4324,7 @@
         <v>290</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -4255,13 +4361,13 @@
         <v>113</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>114</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -4298,13 +4404,13 @@
         <v>113</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -4385,7 +4491,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>219</v>
@@ -4422,7 +4528,7 @@
         <v>122</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="4"/>
@@ -4457,7 +4563,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>220</v>
@@ -4519,7 +4625,7 @@
         <v>122</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="4"/>
@@ -5304,7 +5410,7 @@
         <v>10</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I33" s="16" t="s">
         <v>183</v>
@@ -5327,7 +5433,7 @@
         <v>10</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I34" s="16" t="s">
         <v>184</v>
@@ -5413,7 +5519,7 @@
         <v>111</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F38" s="16" t="s">
         <v>177</v>
@@ -5459,10 +5565,10 @@
         <v>228</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -5496,7 +5602,7 @@
         <v>301</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D42" s="16" t="s">
         <v>227</v>
@@ -5508,7 +5614,7 @@
         <v>196</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I42" s="16" t="s">
         <v>197</v>

</xml_diff>